<commit_message>
update data for 2022-05-07
</commit_message>
<xml_diff>
--- a/data/proceed/BJFK_20220507_addr.xlsx
+++ b/data/proceed/BJFK_20220507_addr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="756" uniqueCount="343">
   <si>
     <t>状态</t>
   </si>
@@ -412,6 +412,9 @@
     <t>亦庄镇南海雅苑北区20号楼(4月28日0时起)</t>
   </si>
   <si>
+    <t>亦庄镇南海雅苑北区2号楼底商小荷鲜生店铺(4月28日0时起)</t>
+  </si>
+  <si>
     <t>采育镇前甫村、后甫村(4月29日20时起)</t>
   </si>
   <si>
@@ -953,6 +956,9 @@
   </si>
   <si>
     <t>大兴区亦庄镇南海雅苑北区20号楼</t>
+  </si>
+  <si>
+    <t>大兴区亦庄镇南海雅苑北区2号楼底商小荷鲜生店铺</t>
   </si>
   <si>
     <t>大兴区采育镇前甫村、后甫村</t>
@@ -1394,7 +1400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D188"/>
+  <dimension ref="A1:D189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1425,7 +1431,7 @@
         <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1439,7 +1445,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1453,7 +1459,7 @@
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1467,7 +1473,7 @@
         <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1481,7 +1487,7 @@
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1495,7 +1501,7 @@
         <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1509,7 +1515,7 @@
         <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1523,7 +1529,7 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1537,7 +1543,7 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1551,7 +1557,7 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1565,7 +1571,7 @@
         <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1579,7 +1585,7 @@
         <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1593,7 +1599,7 @@
         <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1607,7 +1613,7 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1621,7 +1627,7 @@
         <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1635,7 +1641,7 @@
         <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1649,7 +1655,7 @@
         <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1663,7 +1669,7 @@
         <v>26</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1677,7 +1683,7 @@
         <v>27</v>
       </c>
       <c r="D20" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1691,7 +1697,7 @@
         <v>28</v>
       </c>
       <c r="D21" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1705,7 +1711,7 @@
         <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1719,7 +1725,7 @@
         <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1733,7 +1739,7 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1747,7 +1753,7 @@
         <v>32</v>
       </c>
       <c r="D25" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1761,7 +1767,7 @@
         <v>33</v>
       </c>
       <c r="D26" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1775,7 +1781,7 @@
         <v>34</v>
       </c>
       <c r="D27" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1789,7 +1795,7 @@
         <v>35</v>
       </c>
       <c r="D28" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1803,7 +1809,7 @@
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1817,7 +1823,7 @@
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1831,7 +1837,7 @@
         <v>36</v>
       </c>
       <c r="D31" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1845,7 +1851,7 @@
         <v>37</v>
       </c>
       <c r="D32" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1859,7 +1865,7 @@
         <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1873,7 +1879,7 @@
         <v>39</v>
       </c>
       <c r="D34" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1887,7 +1893,7 @@
         <v>39</v>
       </c>
       <c r="D35" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1901,7 +1907,7 @@
         <v>40</v>
       </c>
       <c r="D36" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1915,7 +1921,7 @@
         <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1929,7 +1935,7 @@
         <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1943,7 +1949,7 @@
         <v>42</v>
       </c>
       <c r="D39" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1957,7 +1963,7 @@
         <v>43</v>
       </c>
       <c r="D40" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1971,7 +1977,7 @@
         <v>43</v>
       </c>
       <c r="D41" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1985,7 +1991,7 @@
         <v>43</v>
       </c>
       <c r="D42" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1999,7 +2005,7 @@
         <v>44</v>
       </c>
       <c r="D43" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2013,7 +2019,7 @@
         <v>45</v>
       </c>
       <c r="D44" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2027,7 +2033,7 @@
         <v>46</v>
       </c>
       <c r="D45" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2041,7 +2047,7 @@
         <v>47</v>
       </c>
       <c r="D46" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2055,7 +2061,7 @@
         <v>48</v>
       </c>
       <c r="D47" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2069,7 +2075,7 @@
         <v>48</v>
       </c>
       <c r="D48" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2083,7 +2089,7 @@
         <v>49</v>
       </c>
       <c r="D49" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2097,7 +2103,7 @@
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2111,7 +2117,7 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2125,7 +2131,7 @@
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2139,7 +2145,7 @@
         <v>51</v>
       </c>
       <c r="D53" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2153,7 +2159,7 @@
         <v>52</v>
       </c>
       <c r="D54" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2167,7 +2173,7 @@
         <v>53</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2181,7 +2187,7 @@
         <v>54</v>
       </c>
       <c r="D56" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2195,7 +2201,7 @@
         <v>55</v>
       </c>
       <c r="D57" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2209,7 +2215,7 @@
         <v>56</v>
       </c>
       <c r="D58" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2223,7 +2229,7 @@
         <v>57</v>
       </c>
       <c r="D59" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2237,7 +2243,7 @@
         <v>58</v>
       </c>
       <c r="D60" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2251,7 +2257,7 @@
         <v>59</v>
       </c>
       <c r="D61" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2265,7 +2271,7 @@
         <v>60</v>
       </c>
       <c r="D62" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2279,7 +2285,7 @@
         <v>61</v>
       </c>
       <c r="D63" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2293,7 +2299,7 @@
         <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2307,7 +2313,7 @@
         <v>63</v>
       </c>
       <c r="D65" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2321,7 +2327,7 @@
         <v>64</v>
       </c>
       <c r="D66" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2335,7 +2341,7 @@
         <v>65</v>
       </c>
       <c r="D67" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2349,7 +2355,7 @@
         <v>66</v>
       </c>
       <c r="D68" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2363,7 +2369,7 @@
         <v>67</v>
       </c>
       <c r="D69" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2377,7 +2383,7 @@
         <v>68</v>
       </c>
       <c r="D70" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2391,7 +2397,7 @@
         <v>69</v>
       </c>
       <c r="D71" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2405,7 +2411,7 @@
         <v>69</v>
       </c>
       <c r="D72" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2419,7 +2425,7 @@
         <v>69</v>
       </c>
       <c r="D73" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2433,7 +2439,7 @@
         <v>69</v>
       </c>
       <c r="D74" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2447,7 +2453,7 @@
         <v>70</v>
       </c>
       <c r="D75" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2461,7 +2467,7 @@
         <v>71</v>
       </c>
       <c r="D76" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2475,7 +2481,7 @@
         <v>72</v>
       </c>
       <c r="D77" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2489,7 +2495,7 @@
         <v>73</v>
       </c>
       <c r="D78" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2503,7 +2509,7 @@
         <v>74</v>
       </c>
       <c r="D79" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2517,7 +2523,7 @@
         <v>74</v>
       </c>
       <c r="D80" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2531,7 +2537,7 @@
         <v>75</v>
       </c>
       <c r="D81" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2545,7 +2551,7 @@
         <v>76</v>
       </c>
       <c r="D82" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="1:4">
@@ -2559,7 +2565,7 @@
         <v>77</v>
       </c>
       <c r="D83" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2573,7 +2579,7 @@
         <v>77</v>
       </c>
       <c r="D84" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -2587,7 +2593,7 @@
         <v>77</v>
       </c>
       <c r="D85" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -2601,7 +2607,7 @@
         <v>77</v>
       </c>
       <c r="D86" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -2615,7 +2621,7 @@
         <v>77</v>
       </c>
       <c r="D87" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -2629,7 +2635,7 @@
         <v>77</v>
       </c>
       <c r="D88" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -2643,7 +2649,7 @@
         <v>77</v>
       </c>
       <c r="D89" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -2657,7 +2663,7 @@
         <v>77</v>
       </c>
       <c r="D90" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -2671,7 +2677,7 @@
         <v>77</v>
       </c>
       <c r="D91" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2685,7 +2691,7 @@
         <v>78</v>
       </c>
       <c r="D92" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -2699,7 +2705,7 @@
         <v>79</v>
       </c>
       <c r="D93" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -2713,7 +2719,7 @@
         <v>79</v>
       </c>
       <c r="D94" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2727,7 +2733,7 @@
         <v>79</v>
       </c>
       <c r="D95" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2741,7 +2747,7 @@
         <v>80</v>
       </c>
       <c r="D96" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -2755,7 +2761,7 @@
         <v>81</v>
       </c>
       <c r="D97" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2769,7 +2775,7 @@
         <v>82</v>
       </c>
       <c r="D98" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2783,7 +2789,7 @@
         <v>83</v>
       </c>
       <c r="D99" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2797,7 +2803,7 @@
         <v>84</v>
       </c>
       <c r="D100" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2811,7 +2817,7 @@
         <v>85</v>
       </c>
       <c r="D101" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2825,7 +2831,7 @@
         <v>86</v>
       </c>
       <c r="D102" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2839,7 +2845,7 @@
         <v>86</v>
       </c>
       <c r="D103" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -2853,7 +2859,7 @@
         <v>86</v>
       </c>
       <c r="D104" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -2867,7 +2873,7 @@
         <v>86</v>
       </c>
       <c r="D105" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2881,7 +2887,7 @@
         <v>86</v>
       </c>
       <c r="D106" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -2895,7 +2901,7 @@
         <v>86</v>
       </c>
       <c r="D107" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2909,7 +2915,7 @@
         <v>86</v>
       </c>
       <c r="D108" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -2923,7 +2929,7 @@
         <v>86</v>
       </c>
       <c r="D109" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -2937,7 +2943,7 @@
         <v>86</v>
       </c>
       <c r="D110" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -2951,7 +2957,7 @@
         <v>86</v>
       </c>
       <c r="D111" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2965,7 +2971,7 @@
         <v>86</v>
       </c>
       <c r="D112" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -2979,7 +2985,7 @@
         <v>87</v>
       </c>
       <c r="D113" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -2993,7 +2999,7 @@
         <v>88</v>
       </c>
       <c r="D114" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3007,7 +3013,7 @@
         <v>89</v>
       </c>
       <c r="D115" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3021,7 +3027,7 @@
         <v>89</v>
       </c>
       <c r="D116" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3035,7 +3041,7 @@
         <v>90</v>
       </c>
       <c r="D117" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3049,7 +3055,7 @@
         <v>91</v>
       </c>
       <c r="D118" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3063,7 +3069,7 @@
         <v>92</v>
       </c>
       <c r="D119" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3077,7 +3083,7 @@
         <v>93</v>
       </c>
       <c r="D120" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3091,7 +3097,7 @@
         <v>94</v>
       </c>
       <c r="D121" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3105,7 +3111,7 @@
         <v>95</v>
       </c>
       <c r="D122" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3119,7 +3125,7 @@
         <v>96</v>
       </c>
       <c r="D123" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3133,7 +3139,7 @@
         <v>97</v>
       </c>
       <c r="D124" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3147,7 +3153,7 @@
         <v>98</v>
       </c>
       <c r="D125" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3161,7 +3167,7 @@
         <v>99</v>
       </c>
       <c r="D126" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3175,7 +3181,7 @@
         <v>100</v>
       </c>
       <c r="D127" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3189,7 +3195,7 @@
         <v>101</v>
       </c>
       <c r="D128" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3203,7 +3209,7 @@
         <v>102</v>
       </c>
       <c r="D129" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3217,7 +3223,7 @@
         <v>103</v>
       </c>
       <c r="D130" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3231,7 +3237,7 @@
         <v>104</v>
       </c>
       <c r="D131" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3245,7 +3251,7 @@
         <v>105</v>
       </c>
       <c r="D132" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3259,7 +3265,7 @@
         <v>106</v>
       </c>
       <c r="D133" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3273,7 +3279,7 @@
         <v>107</v>
       </c>
       <c r="D134" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3287,7 +3293,7 @@
         <v>108</v>
       </c>
       <c r="D135" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3301,7 +3307,7 @@
         <v>109</v>
       </c>
       <c r="D136" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -3315,7 +3321,7 @@
         <v>110</v>
       </c>
       <c r="D137" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -3329,7 +3335,7 @@
         <v>111</v>
       </c>
       <c r="D138" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3343,7 +3349,7 @@
         <v>112</v>
       </c>
       <c r="D139" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3357,7 +3363,7 @@
         <v>113</v>
       </c>
       <c r="D140" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3371,7 +3377,7 @@
         <v>114</v>
       </c>
       <c r="D141" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3385,7 +3391,7 @@
         <v>115</v>
       </c>
       <c r="D142" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3399,7 +3405,7 @@
         <v>116</v>
       </c>
       <c r="D143" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3413,7 +3419,7 @@
         <v>117</v>
       </c>
       <c r="D144" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3427,7 +3433,7 @@
         <v>118</v>
       </c>
       <c r="D145" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3441,7 +3447,7 @@
         <v>118</v>
       </c>
       <c r="D146" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3455,7 +3461,7 @@
         <v>118</v>
       </c>
       <c r="D147" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3469,7 +3475,7 @@
         <v>119</v>
       </c>
       <c r="D148" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3483,7 +3489,7 @@
         <v>120</v>
       </c>
       <c r="D149" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3497,7 +3503,7 @@
         <v>121</v>
       </c>
       <c r="D150" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3511,7 +3517,7 @@
         <v>122</v>
       </c>
       <c r="D151" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="152" spans="1:4">
@@ -3525,7 +3531,7 @@
         <v>123</v>
       </c>
       <c r="D152" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3539,7 +3545,7 @@
         <v>124</v>
       </c>
       <c r="D153" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="154" spans="1:4">
@@ -3553,7 +3559,7 @@
         <v>125</v>
       </c>
       <c r="D154" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3567,7 +3573,7 @@
         <v>126</v>
       </c>
       <c r="D155" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3581,7 +3587,7 @@
         <v>127</v>
       </c>
       <c r="D156" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -3595,7 +3601,7 @@
         <v>128</v>
       </c>
       <c r="D157" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -3609,7 +3615,7 @@
         <v>129</v>
       </c>
       <c r="D158" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3623,7 +3629,7 @@
         <v>130</v>
       </c>
       <c r="D159" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3637,7 +3643,7 @@
         <v>131</v>
       </c>
       <c r="D160" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3651,7 +3657,7 @@
         <v>132</v>
       </c>
       <c r="D161" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -3665,7 +3671,7 @@
         <v>133</v>
       </c>
       <c r="D162" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -3679,7 +3685,7 @@
         <v>134</v>
       </c>
       <c r="D163" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -3687,13 +3693,13 @@
         <v>4</v>
       </c>
       <c r="B164" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C164" t="s">
         <v>135</v>
       </c>
       <c r="D164" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -3701,13 +3707,13 @@
         <v>4</v>
       </c>
       <c r="B165" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C165" t="s">
         <v>136</v>
       </c>
       <c r="D165" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -3715,13 +3721,13 @@
         <v>4</v>
       </c>
       <c r="B166" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C166" t="s">
         <v>137</v>
       </c>
       <c r="D166" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -3735,7 +3741,7 @@
         <v>138</v>
       </c>
       <c r="D167" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3743,13 +3749,13 @@
         <v>4</v>
       </c>
       <c r="B168" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C168" t="s">
         <v>139</v>
       </c>
       <c r="D168" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -3763,7 +3769,7 @@
         <v>140</v>
       </c>
       <c r="D169" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -3777,7 +3783,7 @@
         <v>141</v>
       </c>
       <c r="D170" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -3791,7 +3797,7 @@
         <v>142</v>
       </c>
       <c r="D171" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -3802,10 +3808,10 @@
         <v>15</v>
       </c>
       <c r="C172" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D172" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -3816,10 +3822,10 @@
         <v>15</v>
       </c>
       <c r="C173" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D173" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -3830,10 +3836,10 @@
         <v>15</v>
       </c>
       <c r="C174" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D174" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -3844,10 +3850,10 @@
         <v>15</v>
       </c>
       <c r="C175" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D175" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -3858,10 +3864,10 @@
         <v>15</v>
       </c>
       <c r="C176" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D176" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -3875,7 +3881,7 @@
         <v>143</v>
       </c>
       <c r="D177" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -3889,7 +3895,7 @@
         <v>144</v>
       </c>
       <c r="D178" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="179" spans="1:4">
@@ -3903,7 +3909,7 @@
         <v>145</v>
       </c>
       <c r="D179" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -3917,7 +3923,7 @@
         <v>146</v>
       </c>
       <c r="D180" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -3931,7 +3937,7 @@
         <v>147</v>
       </c>
       <c r="D181" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -3945,7 +3951,7 @@
         <v>148</v>
       </c>
       <c r="D182" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -3959,7 +3965,7 @@
         <v>149</v>
       </c>
       <c r="D183" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -3973,7 +3979,7 @@
         <v>150</v>
       </c>
       <c r="D184" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -3981,13 +3987,13 @@
         <v>4</v>
       </c>
       <c r="B185" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C185" t="s">
         <v>151</v>
       </c>
       <c r="D185" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4001,7 +4007,7 @@
         <v>152</v>
       </c>
       <c r="D186" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4009,13 +4015,13 @@
         <v>4</v>
       </c>
       <c r="B187" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C187" t="s">
         <v>153</v>
       </c>
       <c r="D187" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="188" spans="1:4">
@@ -4023,13 +4029,27 @@
         <v>4</v>
       </c>
       <c r="B188" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C188" t="s">
         <v>154</v>
       </c>
       <c r="D188" t="s">
-        <v>340</v>
+        <v>341</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
+      <c r="A189" t="s">
+        <v>4</v>
+      </c>
+      <c r="B189" t="s">
+        <v>18</v>
+      </c>
+      <c r="C189" t="s">
+        <v>155</v>
+      </c>
+      <c r="D189" t="s">
+        <v>342</v>
       </c>
     </row>
   </sheetData>

</xml_diff>